<commit_message>
insert chmi hydro stations to database
</commit_message>
<xml_diff>
--- a/hydrodatainfo/metadata/chmi_hydro_stations.xlsx
+++ b/hydrodatainfo/metadata/chmi_hydro_stations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="503">
   <si>
     <t>Hracholusky</t>
   </si>
@@ -1522,6 +1522,9 @@
   </si>
   <si>
     <t>Stříbrný potok</t>
+  </si>
+  <si>
+    <t>NEW</t>
   </si>
 </sst>
 </file>
@@ -1864,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C338"/>
+  <dimension ref="A1:D338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="G337" sqref="G337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1881,7 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>307247</v>
       </c>
@@ -1888,8 +1891,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>307073</v>
       </c>
@@ -1899,8 +1905,11 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2505265</v>
       </c>
@@ -1910,8 +1919,11 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2505266</v>
       </c>
@@ -1921,8 +1933,11 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2505267</v>
       </c>
@@ -1932,8 +1947,11 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2505270</v>
       </c>
@@ -1943,8 +1961,11 @@
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>307036</v>
       </c>
@@ -1954,8 +1975,11 @@
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>307038</v>
       </c>
@@ -1965,8 +1989,11 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>307056</v>
       </c>
@@ -1976,8 +2003,11 @@
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2505272</v>
       </c>
@@ -1987,8 +2017,11 @@
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2505280</v>
       </c>
@@ -1998,8 +2031,11 @@
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2505281</v>
       </c>
@@ -2009,8 +2045,11 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2505283</v>
       </c>
@@ -2020,8 +2059,11 @@
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2505286</v>
       </c>
@@ -2031,8 +2073,11 @@
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2505290</v>
       </c>
@@ -2042,8 +2087,11 @@
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2505294</v>
       </c>
@@ -2053,8 +2101,11 @@
       <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2506441</v>
       </c>
@@ -2064,8 +2115,11 @@
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2506445</v>
       </c>
@@ -2075,8 +2129,11 @@
       <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2535576</v>
       </c>
@@ -2086,8 +2143,11 @@
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>307032</v>
       </c>
@@ -2097,8 +2157,11 @@
       <c r="C20" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>307071</v>
       </c>
@@ -2108,8 +2171,11 @@
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>307319</v>
       </c>
@@ -2119,8 +2185,11 @@
       <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>307306</v>
       </c>
@@ -2130,8 +2199,11 @@
       <c r="C23" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>307322</v>
       </c>
@@ -2141,8 +2213,11 @@
       <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>307351</v>
       </c>
@@ -2152,8 +2227,11 @@
       <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>307357</v>
       </c>
@@ -2163,8 +2241,11 @@
       <c r="C26" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>306989</v>
       </c>
@@ -2174,8 +2255,11 @@
       <c r="C27" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>307124</v>
       </c>
@@ -2185,8 +2269,11 @@
       <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>307129</v>
       </c>
@@ -2196,8 +2283,11 @@
       <c r="C29" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>307139</v>
       </c>
@@ -2207,8 +2297,11 @@
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>307158</v>
       </c>
@@ -2218,8 +2311,11 @@
       <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>307165</v>
       </c>
@@ -2229,8 +2325,11 @@
       <c r="C32" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>307174</v>
       </c>
@@ -2240,8 +2339,11 @@
       <c r="C33" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>307178</v>
       </c>
@@ -2251,8 +2353,11 @@
       <c r="C34" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>307188</v>
       </c>
@@ -2262,8 +2367,11 @@
       <c r="C35" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>307203</v>
       </c>
@@ -2273,8 +2381,11 @@
       <c r="C36" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>307223</v>
       </c>
@@ -2284,8 +2395,11 @@
       <c r="C37" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>307228</v>
       </c>
@@ -2295,8 +2409,11 @@
       <c r="C38" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>307233</v>
       </c>
@@ -2306,8 +2423,11 @@
       <c r="C39" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>307238</v>
       </c>
@@ -2317,8 +2437,11 @@
       <c r="C40" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>307243</v>
       </c>
@@ -2328,8 +2451,11 @@
       <c r="C41" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>307064</v>
       </c>
@@ -2339,8 +2465,11 @@
       <c r="C42" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>307145</v>
       </c>
@@ -2350,8 +2479,11 @@
       <c r="C43" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>307348</v>
       </c>
@@ -2361,8 +2493,11 @@
       <c r="C44" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>306992</v>
       </c>
@@ -2372,8 +2507,11 @@
       <c r="C45" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>307011</v>
       </c>
@@ -2383,8 +2521,11 @@
       <c r="C46" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>307044</v>
       </c>
@@ -2394,8 +2535,11 @@
       <c r="C47" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>307092</v>
       </c>
@@ -2405,8 +2549,11 @@
       <c r="C48" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>307107</v>
       </c>
@@ -2416,8 +2563,11 @@
       <c r="C49" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>307193</v>
       </c>
@@ -2427,8 +2577,11 @@
       <c r="C50" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>307210</v>
       </c>
@@ -2438,8 +2591,11 @@
       <c r="C51" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>306976</v>
       </c>
@@ -2449,8 +2605,11 @@
       <c r="C52" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>306978</v>
       </c>
@@ -2460,8 +2619,11 @@
       <c r="C53" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>306990</v>
       </c>
@@ -2471,8 +2633,11 @@
       <c r="C54" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>307005</v>
       </c>
@@ -2482,8 +2647,11 @@
       <c r="C55" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>307009</v>
       </c>
@@ -2493,8 +2661,11 @@
       <c r="C56" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="2">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>307058</v>
       </c>
@@ -2504,8 +2675,11 @@
       <c r="C57" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>307068</v>
       </c>
@@ -2515,8 +2689,11 @@
       <c r="C58" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>307076</v>
       </c>
@@ -2526,8 +2703,11 @@
       <c r="C59" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>307099</v>
       </c>
@@ -2537,8 +2717,11 @@
       <c r="C60" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="2">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>307118</v>
       </c>
@@ -2548,8 +2731,11 @@
       <c r="C61" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>307096</v>
       </c>
@@ -2559,8 +2745,11 @@
       <c r="C62" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>307100</v>
       </c>
@@ -2570,8 +2759,11 @@
       <c r="C63" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>307105</v>
       </c>
@@ -2581,8 +2773,11 @@
       <c r="C64" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>307110</v>
       </c>
@@ -2592,8 +2787,11 @@
       <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>307116</v>
       </c>
@@ -2603,8 +2801,11 @@
       <c r="C66" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>307132</v>
       </c>
@@ -2614,8 +2815,11 @@
       <c r="C67" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>307146</v>
       </c>
@@ -2625,8 +2829,11 @@
       <c r="C68" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="2">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>307147</v>
       </c>
@@ -2636,8 +2843,11 @@
       <c r="C69" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>307160</v>
       </c>
@@ -2647,8 +2857,11 @@
       <c r="C70" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>307366</v>
       </c>
@@ -2658,8 +2871,11 @@
       <c r="C71" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>307126</v>
       </c>
@@ -2669,8 +2885,11 @@
       <c r="C72" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>307151</v>
       </c>
@@ -2680,8 +2899,11 @@
       <c r="C73" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>307184</v>
       </c>
@@ -2691,8 +2913,11 @@
       <c r="C74" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="2">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>307219</v>
       </c>
@@ -2702,8 +2927,11 @@
       <c r="C75" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="2">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>307225</v>
       </c>
@@ -2713,8 +2941,11 @@
       <c r="C76" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>307239</v>
       </c>
@@ -2724,8 +2955,11 @@
       <c r="C77" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>307244</v>
       </c>
@@ -2735,8 +2969,11 @@
       <c r="C78" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="2">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>307255</v>
       </c>
@@ -2746,8 +2983,11 @@
       <c r="C79" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>307265</v>
       </c>
@@ -2757,8 +2997,11 @@
       <c r="C80" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>307273</v>
       </c>
@@ -2768,8 +3011,11 @@
       <c r="C81" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>307297</v>
       </c>
@@ -2779,8 +3025,11 @@
       <c r="C82" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>307313</v>
       </c>
@@ -2790,8 +3039,11 @@
       <c r="C83" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>307316</v>
       </c>
@@ -2801,8 +3053,11 @@
       <c r="C84" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>307337</v>
       </c>
@@ -2812,8 +3067,11 @@
       <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>307350</v>
       </c>
@@ -2823,8 +3081,11 @@
       <c r="C86" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="2">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>307355</v>
       </c>
@@ -2834,8 +3095,11 @@
       <c r="C87" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>307370</v>
       </c>
@@ -2845,8 +3109,11 @@
       <c r="C88" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>307176</v>
       </c>
@@ -2856,8 +3123,11 @@
       <c r="C89" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>307365</v>
       </c>
@@ -2867,8 +3137,11 @@
       <c r="C90" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="2">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>2586337</v>
       </c>
@@ -2878,8 +3151,11 @@
       <c r="C91" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2505260</v>
       </c>
@@ -2889,8 +3165,11 @@
       <c r="C92" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>2605340</v>
       </c>
@@ -2900,8 +3179,11 @@
       <c r="C93" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="2">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>307343</v>
       </c>
@@ -2911,8 +3193,11 @@
       <c r="C94" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="2">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>307352</v>
       </c>
@@ -2922,8 +3207,11 @@
       <c r="C95" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>307017</v>
       </c>
@@ -2933,8 +3221,11 @@
       <c r="C96" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>307119</v>
       </c>
@@ -2944,8 +3235,11 @@
       <c r="C97" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="2">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>307137</v>
       </c>
@@ -2955,8 +3249,11 @@
       <c r="C98" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>307155</v>
       </c>
@@ -2966,8 +3263,11 @@
       <c r="C99" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>307186</v>
       </c>
@@ -2977,8 +3277,11 @@
       <c r="C100" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="2">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>307197</v>
       </c>
@@ -2988,8 +3291,11 @@
       <c r="C101" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>307217</v>
       </c>
@@ -2999,8 +3305,11 @@
       <c r="C102" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>307221</v>
       </c>
@@ -3010,8 +3319,11 @@
       <c r="C103" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="2">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>306974</v>
       </c>
@@ -3021,8 +3333,11 @@
       <c r="C104" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="2">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>306987</v>
       </c>
@@ -3032,8 +3347,11 @@
       <c r="C105" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>307164</v>
       </c>
@@ -3043,8 +3361,11 @@
       <c r="C106" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>307189</v>
       </c>
@@ -3054,8 +3375,11 @@
       <c r="C107" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>307201</v>
       </c>
@@ -3065,8 +3389,11 @@
       <c r="C108" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>307212</v>
       </c>
@@ -3076,8 +3403,11 @@
       <c r="C109" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>307232</v>
       </c>
@@ -3087,8 +3417,11 @@
       <c r="C110" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>307245</v>
       </c>
@@ -3098,8 +3431,11 @@
       <c r="C111" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>307246</v>
       </c>
@@ -3109,8 +3445,11 @@
       <c r="C112" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>307256</v>
       </c>
@@ -3120,8 +3459,11 @@
       <c r="C113" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" s="2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>307282</v>
       </c>
@@ -3131,8 +3473,11 @@
       <c r="C114" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>307285</v>
       </c>
@@ -3142,8 +3487,11 @@
       <c r="C115" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="2">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>307289</v>
       </c>
@@ -3153,8 +3501,11 @@
       <c r="C116" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>307293</v>
       </c>
@@ -3164,8 +3515,11 @@
       <c r="C117" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="2">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>307300</v>
       </c>
@@ -3175,8 +3529,11 @@
       <c r="C118" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>307304</v>
       </c>
@@ -3186,8 +3543,11 @@
       <c r="C119" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="2">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>307311</v>
       </c>
@@ -3197,8 +3557,11 @@
       <c r="C120" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>307321</v>
       </c>
@@ -3208,8 +3571,11 @@
       <c r="C121" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>307336</v>
       </c>
@@ -3219,8 +3585,11 @@
       <c r="C122" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>307231</v>
       </c>
@@ -3230,8 +3599,11 @@
       <c r="C123" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>307242</v>
       </c>
@@ -3241,8 +3613,11 @@
       <c r="C124" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" s="2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>307253</v>
       </c>
@@ -3252,8 +3627,11 @@
       <c r="C125" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>307258</v>
       </c>
@@ -3263,8 +3641,11 @@
       <c r="C126" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" s="2">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>307267</v>
       </c>
@@ -3274,8 +3655,11 @@
       <c r="C127" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" s="2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>307280</v>
       </c>
@@ -3285,8 +3669,11 @@
       <c r="C128" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" s="2">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>307344</v>
       </c>
@@ -3296,8 +3683,11 @@
       <c r="C129" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="2">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>307371</v>
       </c>
@@ -3307,8 +3697,11 @@
       <c r="C130" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="2">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>306991</v>
       </c>
@@ -3318,8 +3711,11 @@
       <c r="C131" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="2">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>306995</v>
       </c>
@@ -3329,8 +3725,11 @@
       <c r="C132" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" s="2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>306997</v>
       </c>
@@ -3340,8 +3739,11 @@
       <c r="C133" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" s="2">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>307007</v>
       </c>
@@ -3351,8 +3753,11 @@
       <c r="C134" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>307010</v>
       </c>
@@ -3362,8 +3767,11 @@
       <c r="C135" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" s="2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>307027</v>
       </c>
@@ -3373,8 +3781,11 @@
       <c r="C136" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>307047</v>
       </c>
@@ -3384,8 +3795,11 @@
       <c r="C137" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" s="2">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>307060</v>
       </c>
@@ -3395,8 +3809,11 @@
       <c r="C138" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" s="2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>307097</v>
       </c>
@@ -3406,8 +3823,11 @@
       <c r="C139" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>307113</v>
       </c>
@@ -3417,8 +3837,11 @@
       <c r="C140" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" s="2">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>307042</v>
       </c>
@@ -3428,8 +3851,11 @@
       <c r="C141" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" s="2">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>307241</v>
       </c>
@@ -3439,8 +3865,11 @@
       <c r="C142" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>307328</v>
       </c>
@@ -3450,8 +3879,11 @@
       <c r="C143" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" s="2">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>307372</v>
       </c>
@@ -3461,8 +3893,11 @@
       <c r="C144" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" s="2">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>307171</v>
       </c>
@@ -3472,8 +3907,11 @@
       <c r="C145" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>307123</v>
       </c>
@@ -3483,8 +3921,11 @@
       <c r="C146" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>307134</v>
       </c>
@@ -3494,8 +3935,11 @@
       <c r="C147" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" s="2">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>307303</v>
       </c>
@@ -3505,8 +3949,11 @@
       <c r="C148" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" s="2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>307318</v>
       </c>
@@ -3516,8 +3963,11 @@
       <c r="C149" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" s="2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>307353</v>
       </c>
@@ -3527,8 +3977,11 @@
       <c r="C150" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" s="2">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>307215</v>
       </c>
@@ -3538,8 +3991,11 @@
       <c r="C151" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>307046</v>
       </c>
@@ -3549,8 +4005,11 @@
       <c r="C152" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" s="2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>307339</v>
       </c>
@@ -3560,8 +4019,11 @@
       <c r="C153" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" s="2">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>307078</v>
       </c>
@@ -3571,8 +4033,11 @@
       <c r="C154" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" s="2">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>307358</v>
       </c>
@@ -3582,8 +4047,11 @@
       <c r="C155" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" s="2">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>307326</v>
       </c>
@@ -3593,8 +4061,11 @@
       <c r="C156" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" s="2">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>307121</v>
       </c>
@@ -3604,8 +4075,11 @@
       <c r="C157" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" s="2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>307028</v>
       </c>
@@ -3615,8 +4089,11 @@
       <c r="C158" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" s="2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>307360</v>
       </c>
@@ -3626,8 +4103,11 @@
       <c r="C159" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" s="2">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>307152</v>
       </c>
@@ -3637,8 +4117,11 @@
       <c r="C160" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2505277</v>
       </c>
@@ -3648,8 +4131,11 @@
       <c r="C161" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" s="2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>307216</v>
       </c>
@@ -3659,8 +4145,11 @@
       <c r="C162" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" s="2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>306981</v>
       </c>
@@ -3670,8 +4159,11 @@
       <c r="C163" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" s="2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2505258</v>
       </c>
@@ -3681,8 +4173,11 @@
       <c r="C164" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>307127</v>
       </c>
@@ -3692,8 +4187,11 @@
       <c r="C165" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" s="2">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>307091</v>
       </c>
@@ -3703,8 +4201,11 @@
       <c r="C166" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>307235</v>
       </c>
@@ -3714,8 +4215,11 @@
       <c r="C167" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" s="2">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>306985</v>
       </c>
@@ -3725,8 +4229,11 @@
       <c r="C168" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>307000</v>
       </c>
@@ -3736,8 +4243,11 @@
       <c r="C169" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>307049</v>
       </c>
@@ -3747,8 +4257,11 @@
       <c r="C170" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>307080</v>
       </c>
@@ -3758,8 +4271,11 @@
       <c r="C171" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" s="2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>307003</v>
       </c>
@@ -3769,8 +4285,11 @@
       <c r="C172" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" s="2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>307254</v>
       </c>
@@ -3780,8 +4299,11 @@
       <c r="C173" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" s="2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>2497644</v>
       </c>
@@ -3791,8 +4313,11 @@
       <c r="C174" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>2497645</v>
       </c>
@@ -3802,8 +4327,11 @@
       <c r="C175" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175" s="2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>2497648</v>
       </c>
@@ -3813,8 +4341,11 @@
       <c r="C176" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" s="2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>2504743</v>
       </c>
@@ -3824,8 +4355,11 @@
       <c r="C177" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" s="2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>2504744</v>
       </c>
@@ -3835,8 +4369,11 @@
       <c r="C178" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" s="2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>2504745</v>
       </c>
@@ -3846,8 +4383,11 @@
       <c r="C179" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" s="2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2505252</v>
       </c>
@@ -3857,8 +4397,11 @@
       <c r="C180" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" s="2">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2505254</v>
       </c>
@@ -3868,8 +4411,11 @@
       <c r="C181" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" s="2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>307354</v>
       </c>
@@ -3879,8 +4425,11 @@
       <c r="C182" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" s="2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>307363</v>
       </c>
@@ -3890,8 +4439,11 @@
       <c r="C183" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" s="2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>307162</v>
       </c>
@@ -3901,8 +4453,11 @@
       <c r="C184" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" s="2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>307257</v>
       </c>
@@ -3912,8 +4467,11 @@
       <c r="C185" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" s="2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>307308</v>
       </c>
@@ -3923,8 +4481,11 @@
       <c r="C186" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186" s="2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>307019</v>
       </c>
@@ -3934,8 +4495,11 @@
       <c r="C187" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187" s="2">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2505257</v>
       </c>
@@ -3945,8 +4509,11 @@
       <c r="C188" s="1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188" s="2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>307324</v>
       </c>
@@ -3956,8 +4523,11 @@
       <c r="C189" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189" s="2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>307345</v>
       </c>
@@ -3967,8 +4537,11 @@
       <c r="C190" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>307248</v>
       </c>
@@ -3978,8 +4551,11 @@
       <c r="C191" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191" s="2">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>307150</v>
       </c>
@@ -3989,8 +4565,11 @@
       <c r="C192" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192" s="2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>307072</v>
       </c>
@@ -4000,8 +4579,11 @@
       <c r="C193" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>307299</v>
       </c>
@@ -4011,8 +4593,11 @@
       <c r="C194" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194" s="2">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>307043</v>
       </c>
@@ -4022,8 +4607,11 @@
       <c r="C195" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195" s="2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>306983</v>
       </c>
@@ -4033,8 +4621,11 @@
       <c r="C196" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196" s="2">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2505268</v>
       </c>
@@ -4044,8 +4635,11 @@
       <c r="C197" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197" s="2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>307259</v>
       </c>
@@ -4055,8 +4649,11 @@
       <c r="C198" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198" s="2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>10045028</v>
       </c>
@@ -4066,8 +4663,11 @@
       <c r="C199" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199" s="2">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>10045034</v>
       </c>
@@ -4077,8 +4677,11 @@
       <c r="C200" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D200" s="2">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>10058896</v>
       </c>
@@ -4088,8 +4691,11 @@
       <c r="C201" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201" s="2">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>307234</v>
       </c>
@@ -4099,8 +4705,11 @@
       <c r="C202" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D202" s="2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>307196</v>
       </c>
@@ -4110,8 +4719,11 @@
       <c r="C203" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D203" s="2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>307205</v>
       </c>
@@ -4121,8 +4733,11 @@
       <c r="C204" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D204" s="2">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>306971</v>
       </c>
@@ -4132,8 +4747,11 @@
       <c r="C205" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D205" s="2">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>20070411</v>
       </c>
@@ -4143,8 +4761,11 @@
       <c r="C206" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D206" s="2">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>307053</v>
       </c>
@@ -4154,8 +4775,11 @@
       <c r="C207" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D207" s="2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>2505251</v>
       </c>
@@ -4165,8 +4789,11 @@
       <c r="C208" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D208" s="2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>307142</v>
       </c>
@@ -4176,8 +4803,11 @@
       <c r="C209" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D209" s="2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>307098</v>
       </c>
@@ -4187,8 +4817,11 @@
       <c r="C210" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D210" s="2">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>20070907</v>
       </c>
@@ -4198,8 +4831,11 @@
       <c r="C211" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D211" s="2">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>307057</v>
       </c>
@@ -4209,8 +4845,11 @@
       <c r="C212" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D212" s="2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>307274</v>
       </c>
@@ -4220,8 +4859,11 @@
       <c r="C213" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D213" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>20084971</v>
       </c>
@@ -4231,8 +4873,11 @@
       <c r="C214" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D214" s="2">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>20214893</v>
       </c>
@@ -4242,8 +4887,11 @@
       <c r="C215" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D215" s="2">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>20265575</v>
       </c>
@@ -4253,8 +4901,11 @@
       <c r="C216" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D216" s="2">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>20268815</v>
       </c>
@@ -4264,8 +4915,11 @@
       <c r="C217" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D217" s="2">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>307014</v>
       </c>
@@ -4275,8 +4929,11 @@
       <c r="C218" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D218" s="2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>2505295</v>
       </c>
@@ -4286,8 +4943,11 @@
       <c r="C219" s="1" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D219" s="2">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>20474228</v>
       </c>
@@ -4297,8 +4957,11 @@
       <c r="C220" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D220" s="2">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>307206</v>
       </c>
@@ -4308,8 +4971,11 @@
       <c r="C221" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D221" s="2">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>20284461</v>
       </c>
@@ -4319,8 +4985,11 @@
       <c r="C222" s="1" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D222" s="2">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>20427485</v>
       </c>
@@ -4330,8 +4999,11 @@
       <c r="C223" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D223" s="2">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>20491235</v>
       </c>
@@ -4341,8 +5013,11 @@
       <c r="C224" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D224" s="2">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>20491238</v>
       </c>
@@ -4352,8 +5027,11 @@
       <c r="C225" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D225" s="2">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>20045344</v>
       </c>
@@ -4363,8 +5041,11 @@
       <c r="C226" s="1" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D226" s="2">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>20070460</v>
       </c>
@@ -4374,8 +5055,11 @@
       <c r="C227" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D227" s="2">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>20409119</v>
       </c>
@@ -4385,8 +5069,11 @@
       <c r="C228" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D228" s="2">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>20287377</v>
       </c>
@@ -4396,8 +5083,11 @@
       <c r="C229" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D229" s="2">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>20463360</v>
       </c>
@@ -4407,8 +5097,11 @@
       <c r="C230" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D230" s="2">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>20594353</v>
       </c>
@@ -4418,8 +5111,11 @@
       <c r="C231" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D231" s="2">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>307334</v>
       </c>
@@ -4429,8 +5125,11 @@
       <c r="C232" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D232" s="2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>2505282</v>
       </c>
@@ -4440,8 +5139,11 @@
       <c r="C233" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D233" s="2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>307291</v>
       </c>
@@ -4451,8 +5153,11 @@
       <c r="C234" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D234" s="2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>20214815</v>
       </c>
@@ -4462,8 +5167,11 @@
       <c r="C235" s="1" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D235" s="2">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>20214835</v>
       </c>
@@ -4473,8 +5181,11 @@
       <c r="C236" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D236" s="2">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>307156</v>
       </c>
@@ -4484,8 +5195,11 @@
       <c r="C237" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D237" s="2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>307230</v>
       </c>
@@ -4495,8 +5209,11 @@
       <c r="C238" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D238" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>10059505</v>
       </c>
@@ -4506,8 +5223,11 @@
       <c r="C239" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D239" s="2">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>20241095</v>
       </c>
@@ -4517,8 +5237,11 @@
       <c r="C240" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D240" s="2">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>20262955</v>
       </c>
@@ -4528,8 +5251,11 @@
       <c r="C241" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D241" s="2">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>20023346</v>
       </c>
@@ -4539,8 +5265,11 @@
       <c r="C242" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D242" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>20042094</v>
       </c>
@@ -4550,8 +5279,11 @@
       <c r="C243" s="1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D243" s="2">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>307037</v>
       </c>
@@ -4561,8 +5293,11 @@
       <c r="C244" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D244" s="2">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>20267515</v>
       </c>
@@ -4572,8 +5307,11 @@
       <c r="C245" s="1" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D245" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>20284478</v>
       </c>
@@ -4583,8 +5321,11 @@
       <c r="C246" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D246" s="2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>307054</v>
       </c>
@@ -4594,8 +5335,11 @@
       <c r="C247" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D247" s="2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>307059</v>
       </c>
@@ -4605,8 +5349,11 @@
       <c r="C248" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D248" s="2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>20263035</v>
       </c>
@@ -4616,8 +5363,11 @@
       <c r="C249" s="1" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D249" s="2">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>20368223</v>
       </c>
@@ -4627,8 +5377,11 @@
       <c r="C250" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D250" s="2">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>20403255</v>
       </c>
@@ -4638,8 +5391,11 @@
       <c r="C251" s="1" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D251" s="2">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>20519935</v>
       </c>
@@ -4649,8 +5405,11 @@
       <c r="C252" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D252" s="2">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>307237</v>
       </c>
@@ -4660,8 +5419,11 @@
       <c r="C253" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D253" s="2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>2505291</v>
       </c>
@@ -4671,8 +5433,11 @@
       <c r="C254" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D254" s="2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>10044851</v>
       </c>
@@ -4682,8 +5447,11 @@
       <c r="C255" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D255" s="2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>307226</v>
       </c>
@@ -4693,8 +5461,11 @@
       <c r="C256" s="1" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D256" s="2">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>307284</v>
       </c>
@@ -4704,8 +5475,11 @@
       <c r="C257" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D257" s="2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>20084968</v>
       </c>
@@ -4715,8 +5489,11 @@
       <c r="C258" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D258" s="2">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>20491241</v>
       </c>
@@ -4726,8 +5503,11 @@
       <c r="C259" s="1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D259" s="2">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>20578655</v>
       </c>
@@ -4737,8 +5517,11 @@
       <c r="C260" s="1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D260" s="2">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>20578675</v>
       </c>
@@ -4748,8 +5531,11 @@
       <c r="C261" s="1" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D261" s="2">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>307106</v>
       </c>
@@ -4759,8 +5545,11 @@
       <c r="C262" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D262" s="2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>307268</v>
       </c>
@@ -4770,8 +5559,11 @@
       <c r="C263" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D263" s="2">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>20067738</v>
       </c>
@@ -4781,8 +5573,11 @@
       <c r="C264" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D264" s="2">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>20067780</v>
       </c>
@@ -4792,8 +5587,11 @@
       <c r="C265" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D265" s="2">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>307133</v>
       </c>
@@ -4803,8 +5601,11 @@
       <c r="C266" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D266" s="2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>307015</v>
       </c>
@@ -4814,8 +5615,11 @@
       <c r="C267" s="1" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D267" s="2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>307035</v>
       </c>
@@ -4825,8 +5629,11 @@
       <c r="C268" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D268" s="2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>307185</v>
       </c>
@@ -4836,8 +5643,11 @@
       <c r="C269" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D269" s="2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>307183</v>
       </c>
@@ -4847,8 +5657,11 @@
       <c r="C270" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D270" s="2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>2505259</v>
       </c>
@@ -4858,8 +5671,11 @@
       <c r="C271" s="1" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D271" s="2">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>20753443</v>
       </c>
@@ -4869,8 +5685,11 @@
       <c r="C272" s="1" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D272" s="2">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>307024</v>
       </c>
@@ -4880,8 +5699,11 @@
       <c r="C273" s="1" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D273" s="2">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>20753433</v>
       </c>
@@ -4891,8 +5713,11 @@
       <c r="C274" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D274" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>20816815</v>
       </c>
@@ -4902,8 +5727,11 @@
       <c r="C275" s="1" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D275" s="2">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>22182334</v>
       </c>
@@ -4913,8 +5741,11 @@
       <c r="C276" s="1" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D276" s="2">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>22182516</v>
       </c>
@@ -4924,8 +5755,11 @@
       <c r="C277" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D277" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>22554181</v>
       </c>
@@ -4935,8 +5769,11 @@
       <c r="C278" s="1" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D278" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>23048162</v>
       </c>
@@ -4946,8 +5783,11 @@
       <c r="C279" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D279" s="2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>20757820</v>
       </c>
@@ -4957,8 +5797,11 @@
       <c r="C280" s="1" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D280" s="2">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>307109</v>
       </c>
@@ -4968,8 +5811,11 @@
       <c r="C281" s="1" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D281" s="2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>25089941</v>
       </c>
@@ -4979,8 +5825,11 @@
       <c r="C282" s="1" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D282" s="2">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>20812158</v>
       </c>
@@ -4990,8 +5839,11 @@
       <c r="C283" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D283" s="2">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>23851290</v>
       </c>
@@ -5001,8 +5853,11 @@
       <c r="C284" s="1" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D284" s="2">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>20753413</v>
       </c>
@@ -5012,8 +5867,11 @@
       <c r="C285" s="1" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D285" s="2">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>20773803</v>
       </c>
@@ -5023,8 +5881,11 @@
       <c r="C286" s="1" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D286" s="2">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>20797394</v>
       </c>
@@ -5034,8 +5895,11 @@
       <c r="C287" s="1" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D287" s="2">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>20922048</v>
       </c>
@@ -5045,8 +5909,11 @@
       <c r="C288" s="1" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D288" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>25089890</v>
       </c>
@@ -5056,8 +5923,11 @@
       <c r="C289" s="1" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D289" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>20773798</v>
       </c>
@@ -5067,8 +5937,11 @@
       <c r="C290" s="1" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D290" s="2">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>20823334</v>
       </c>
@@ -5078,8 +5951,11 @@
       <c r="C291" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D291" s="2">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>307310</v>
       </c>
@@ -5089,8 +5965,11 @@
       <c r="C292" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D292" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>307312</v>
       </c>
@@ -5100,8 +5979,11 @@
       <c r="C293" s="1" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D293" s="2">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>2505274</v>
       </c>
@@ -5111,8 +5993,11 @@
       <c r="C294" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D294" s="2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>307294</v>
       </c>
@@ -5122,8 +6007,11 @@
       <c r="C295" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D295" s="2">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>306984</v>
       </c>
@@ -5133,8 +6021,11 @@
       <c r="C296" s="1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D296" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>20697921</v>
       </c>
@@ -5144,8 +6035,11 @@
       <c r="C297" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D297" s="2">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>307361</v>
       </c>
@@ -5155,8 +6049,11 @@
       <c r="C298" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D298" s="2">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>307338</v>
       </c>
@@ -5166,8 +6063,11 @@
       <c r="C299" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D299" s="2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>307199</v>
       </c>
@@ -5177,8 +6077,11 @@
       <c r="C300" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D300" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>307136</v>
       </c>
@@ -5188,8 +6091,11 @@
       <c r="C301" s="1" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D301" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>20650888</v>
       </c>
@@ -5199,8 +6105,11 @@
       <c r="C302" s="1" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D302" s="2">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>20745439</v>
       </c>
@@ -5210,8 +6119,11 @@
       <c r="C303" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D303" s="2">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>20753343</v>
       </c>
@@ -5221,8 +6133,11 @@
       <c r="C304" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D304" s="2">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>2505261</v>
       </c>
@@ -5232,8 +6147,11 @@
       <c r="C305" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D305" s="2">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>307135</v>
       </c>
@@ -5243,8 +6161,11 @@
       <c r="C306" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D306" s="2">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>307229</v>
       </c>
@@ -5254,8 +6175,11 @@
       <c r="C307" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D307" s="2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>2505289</v>
       </c>
@@ -5265,8 +6189,11 @@
       <c r="C308" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D308" s="2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>20677475</v>
       </c>
@@ -5276,8 +6203,11 @@
       <c r="C309" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D309" s="2">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>2505253</v>
       </c>
@@ -5287,8 +6217,11 @@
       <c r="C310" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D310" s="2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>20797314</v>
       </c>
@@ -5298,8 +6231,11 @@
       <c r="C311" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D311" s="2">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>20827805</v>
       </c>
@@ -5309,8 +6245,11 @@
       <c r="C312" s="1" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D312" s="2">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>20910742</v>
       </c>
@@ -5320,8 +6259,11 @@
       <c r="C313" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D313" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>20653435</v>
       </c>
@@ -5331,8 +6273,11 @@
       <c r="C314" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D314" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>20827518</v>
       </c>
@@ -5342,8 +6287,11 @@
       <c r="C315" s="1" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D315" s="2">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>307018</v>
       </c>
@@ -5353,8 +6301,11 @@
       <c r="C316" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D316" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>307065</v>
       </c>
@@ -5364,8 +6315,11 @@
       <c r="C317" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D317" s="2">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>20463355</v>
       </c>
@@ -5375,8 +6329,11 @@
       <c r="C318" s="1" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D318" s="2">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>28977095</v>
       </c>
@@ -5386,8 +6343,11 @@
       <c r="C319" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D319" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>29235299</v>
       </c>
@@ -5397,8 +6357,11 @@
       <c r="C320" s="1" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D320" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>2505256</v>
       </c>
@@ -5408,8 +6371,11 @@
       <c r="C321" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D321" s="2">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>2497647</v>
       </c>
@@ -5419,8 +6385,11 @@
       <c r="C322" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D322" s="2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>2586296</v>
       </c>
@@ -5430,8 +6399,11 @@
       <c r="C323" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D323" s="2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>307161</v>
       </c>
@@ -5441,8 +6413,11 @@
       <c r="C324" s="1" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D324" s="2">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>28611217</v>
       </c>
@@ -5452,8 +6427,11 @@
       <c r="C325" s="1" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D325" s="2">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>31395173</v>
       </c>
@@ -5463,8 +6441,11 @@
       <c r="C326" s="1" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D326" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>28733133</v>
       </c>
@@ -5474,8 +6455,11 @@
       <c r="C327" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D327" s="2">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>28733137</v>
       </c>
@@ -5485,8 +6469,11 @@
       <c r="C328" s="1" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D328" s="2">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>307211</v>
       </c>
@@ -5496,8 +6483,11 @@
       <c r="C329" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D329" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>307236</v>
       </c>
@@ -5507,8 +6497,11 @@
       <c r="C330" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D330" s="2">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>20084974</v>
       </c>
@@ -5518,8 +6511,11 @@
       <c r="C331" s="1" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D331" s="2">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>2504741</v>
       </c>
@@ -5529,8 +6525,11 @@
       <c r="C332" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D332" s="2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>29235761</v>
       </c>
@@ -5540,8 +6539,11 @@
       <c r="C333" s="1" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D333" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>29236133</v>
       </c>
@@ -5551,8 +6553,11 @@
       <c r="C334" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D334" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>307325</v>
       </c>
@@ -5562,8 +6567,11 @@
       <c r="C335" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D335" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>29236544</v>
       </c>
@@ -5573,8 +6581,11 @@
       <c r="C336" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D336" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>29954035</v>
       </c>
@@ -5584,8 +6595,11 @@
       <c r="C337" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D337" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>28975955</v>
       </c>
@@ -5594,6 +6608,9 @@
       </c>
       <c r="C338" s="1" t="s">
         <v>501</v>
+      </c>
+      <c r="D338" s="2" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>